<commit_message>
finsih draft for outsourcing
</commit_message>
<xml_diff>
--- a/source/_drafts/outsourcing-product-development/questionnaire.xlsx
+++ b/source/_drafts/outsourcing-product-development/questionnaire.xlsx
@@ -83,7 +83,7 @@
     <t>Ownership</t>
   </si>
   <si>
-    <t>Are we allowed to change the source code by over own, if we want to ?</t>
+    <t>Are we allowed to change the source code by our own, if we want to ?</t>
   </si>
   <si>
     <t>Yes, you can do that any time.</t>
@@ -101,7 +101,7 @@
     <t>How can we get in contact with you during the project ?</t>
   </si>
   <si>
-    <t>How ever you want. There is no restriction, i will get contact data of all involved persons.</t>
+    <t>How ever you want. There is no restriction, you will get contact data of all involved persons.</t>
   </si>
   <si>
     <t>Is it possible to meet you in person ?</t>
@@ -116,7 +116,7 @@
     <t>Immediatly.</t>
   </si>
   <si>
-    <t>How much time do you need in advance if we want to order further jobs ?</t>
+    <t>How much time do you need in advance if we want to give further jobs ?</t>
   </si>
   <si>
     <t>None.</t>
@@ -156,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -168,13 +168,18 @@
       <name val="Helvetica"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +198,12 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -313,50 +324,47 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -380,6 +388,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -396,10 +405,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -593,14 +602,15 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -615,35 +625,29 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -896,14 +900,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1192,7 +1202,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1475,15 +1485,13 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1641" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.8438" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.8516" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
@@ -1771,7 +1779,7 @@
       <c r="G21" s="11"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="14"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="13"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -1781,12 +1789,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A12:A16"/>
     <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>